<commit_message>
futureF for filter and list qr modification
</commit_message>
<xml_diff>
--- a/vertx-pin/zero-wf/src/main/resources/plugin/wf/oob/data/wf.list.qr.xlsx
+++ b/vertx-pin/zero-wf/src/main/resources/plugin/wf/oob/data/wf.list.qr.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lang/zero-cloud/vertx-zero/vertx-pin/zero-wf/src/main/resources/plugin/wf/oob/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713A93AE-5F15-F844-8DE6-41249740A2D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325AD63D-8D49-4C48-AECC-84FA06127303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="22360" xr2:uid="{BC32819D-176D-6D4B-8CEE-9D375DE1CDB6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="74">
   <si>
     <t>key</t>
   </si>
@@ -91,26 +91,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>OPEN_BY</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACCEPTED_BY</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DEFAULT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CLOSE_BY</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CANCEL_BY</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>视图顺序</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -287,31 +271,55 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>V_OPEN_BY</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V_ACCEPTED_BY</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V_DEFAULT</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V_CLOSE_BY</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V_CANCEL_BY</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DEFAULT/RUN</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DEFAULT/DONE</t>
+    <t>open.by</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>accepted.by</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>close.by</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cancel.by</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>run</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>run/open.by</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>run/accepted.by</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>run/DEFAULT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done/close.by</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done/open.by</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done/cancel.by</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>done/DEFAULT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -836,24 +844,24 @@
   <dimension ref="A2:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21"/>
   <cols>
     <col min="1" max="1" width="55.33203125" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.1640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" style="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="57" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="61.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="61.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="59.1640625" style="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" style="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" style="11" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="58.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="53" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="58" style="3" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="28" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="16384" width="10.83203125" style="3"/>
   </cols>
@@ -890,34 +898,34 @@
         <v>14</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="L3" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -931,34 +939,34 @@
         <v>15</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="J4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="L4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:13">
@@ -966,28 +974,28 @@
         <v>5</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>16</v>
+        <v>67</v>
       </c>
       <c r="D5" s="9">
         <v>1005</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F5" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="G5" s="13" t="s">
-        <v>70</v>
-      </c>
       <c r="H5" s="18" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I5" s="18" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="J5" s="18"/>
       <c r="K5" s="18"/>
@@ -999,28 +1007,28 @@
         <v>6</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>17</v>
+        <v>68</v>
       </c>
       <c r="D6" s="9">
         <v>1010</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I6" s="18" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J6" s="18"/>
       <c r="K6" s="18"/>
@@ -1032,36 +1040,36 @@
         <v>7</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="D7" s="9">
         <v>1015</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J7" s="18"/>
       <c r="K7" s="18"/>
       <c r="L7" s="19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="M7" s="18" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:13">
@@ -1069,28 +1077,28 @@
         <v>8</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>19</v>
+        <v>70</v>
       </c>
       <c r="D8" s="14">
         <v>1005</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="I8" s="18" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="J8" s="18"/>
       <c r="K8" s="18"/>
@@ -1102,28 +1110,28 @@
         <v>9</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="D9" s="15">
         <v>1010</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I9" s="18" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="J9" s="18"/>
       <c r="K9" s="18"/>
@@ -1135,28 +1143,28 @@
         <v>10</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
       <c r="D10" s="15">
         <v>1015</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="J10" s="18"/>
       <c r="K10" s="18"/>
@@ -1168,36 +1176,36 @@
         <v>11</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="D11" s="9">
         <v>1020</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J11" s="18"/>
       <c r="K11" s="18"/>
       <c r="L11" s="19" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="M11" s="18" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>